<commit_message>
com a coluna tipo first e last name
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INTECELERI\Documents\code\automa-o_contas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80F0028-EFA6-4B37-8000-206A8FB8A87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B5F586-489E-413D-B58E-5C0DC1984725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D23106FE-8AF5-4EFE-A13A-AB4EB62D6A66}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>abigail Pinheiro Moraes</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Adenildon OLIVEIRA Ferreira</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>ALUNO</t>
   </si>
 </sst>
 </file>
@@ -406,62 +415,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370D731A-89D7-4DA1-AFAD-7B6A27FB9BE7}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>